<commit_message>
updated scripts to truncate table first before insertion
</commit_message>
<xml_diff>
--- a/_metadesc/parse-page-result.xlsx
+++ b/_metadesc/parse-page-result.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\langkung\fuelcycle\_metadesc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1106C3A6-F1F1-460A-A2EB-5018419988BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2766417-8C3A-453A-927E-B89BE99EC7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="m" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -208,10 +208,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -526,15 +528,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFD26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="53.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="154.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="256" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>